<commit_message>
Revert Data_processed to state before dataset formatting
</commit_message>
<xml_diff>
--- a/Data_processed/electricity/electricity general industry.xlsx
+++ b/Data_processed/electricity/electricity general industry.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:CW3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,20 +446,495 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>..1</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>..2</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>unit</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>process</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>total</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>eco-costs of</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>eco-costs of.1</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>eco-costs of.2</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>eco-costs of.3</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>unnamed: 11</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>unnamed: 12</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>unnamed: 13</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>unnamed: 14</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>human</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>human tox</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>ecotoxicity</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>metals</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>plastic</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>fossil tra</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>biodiversity</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>unnamed: 22</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>unnamed: 23</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>carbon</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>ced</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>non-renewable</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>non-renewable.1</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>non-renewable.2</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>renewable</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>renewable.1</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>renewable.2</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
+          <t>recipe2016</t>
+        </is>
+      </c>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
+          <t>recipe</t>
+        </is>
+      </c>
+      <c r="AI1" s="1" t="inlineStr">
+        <is>
+          <t>recipe.1</t>
+        </is>
+      </c>
+      <c r="AJ1" s="1" t="inlineStr">
+        <is>
+          <t>recipe.2</t>
+        </is>
+      </c>
+      <c r="AK1" s="1" t="inlineStr">
+        <is>
+          <t>recipe.3</t>
+        </is>
+      </c>
+      <c r="AL1" s="1" t="inlineStr">
+        <is>
+          <t>recipe.4</t>
+        </is>
+      </c>
+      <c r="AM1" s="1" t="inlineStr">
+        <is>
+          <t>recipe.5</t>
+        </is>
+      </c>
+      <c r="AN1" s="1" t="inlineStr">
+        <is>
+          <t>global warming,</t>
+        </is>
+      </c>
+      <c r="AO1" s="1" t="inlineStr">
+        <is>
+          <t>global warming, .1</t>
+        </is>
+      </c>
+      <c r="AP1" s="1" t="inlineStr">
+        <is>
+          <t>global warming, .2</t>
+        </is>
+      </c>
+      <c r="AQ1" s="1" t="inlineStr">
+        <is>
+          <t>stratospheric</t>
+        </is>
+      </c>
+      <c r="AR1" s="1" t="inlineStr">
+        <is>
+          <t>ionizing</t>
+        </is>
+      </c>
+      <c r="AS1" s="1" t="inlineStr">
+        <is>
+          <t>ozone formation,</t>
+        </is>
+      </c>
+      <c r="AT1" s="1" t="inlineStr">
+        <is>
+          <t>fine particulate</t>
+        </is>
+      </c>
+      <c r="AU1" s="1" t="inlineStr">
+        <is>
+          <t>ozone formation, .1</t>
+        </is>
+      </c>
+      <c r="AV1" s="1" t="inlineStr">
+        <is>
+          <t>terrestrial</t>
+        </is>
+      </c>
+      <c r="AW1" s="1" t="inlineStr">
+        <is>
+          <t>freshwater</t>
+        </is>
+      </c>
+      <c r="AX1" s="1" t="inlineStr">
+        <is>
+          <t>marine</t>
+        </is>
+      </c>
+      <c r="AY1" s="1" t="inlineStr">
+        <is>
+          <t>terrestrial</t>
+        </is>
+      </c>
+      <c r="AZ1" s="1" t="inlineStr">
+        <is>
+          <t>freshwater</t>
+        </is>
+      </c>
+      <c r="BA1" s="1" t="inlineStr">
+        <is>
+          <t>marine</t>
+        </is>
+      </c>
+      <c r="BB1" s="1" t="inlineStr">
+        <is>
+          <t>human .1</t>
+        </is>
+      </c>
+      <c r="BC1" s="1" t="inlineStr">
+        <is>
+          <t>human .2</t>
+        </is>
+      </c>
+      <c r="BD1" s="1" t="inlineStr">
+        <is>
+          <t>land use</t>
+        </is>
+      </c>
+      <c r="BE1" s="1" t="inlineStr">
+        <is>
+          <t>mineral resource</t>
+        </is>
+      </c>
+      <c r="BF1" s="1" t="inlineStr">
+        <is>
+          <t>fossil resource</t>
+        </is>
+      </c>
+      <c r="BG1" s="1" t="inlineStr">
+        <is>
+          <t>water consumption,</t>
+        </is>
+      </c>
+      <c r="BH1" s="1" t="inlineStr">
+        <is>
+          <t>water consumption,</t>
+        </is>
+      </c>
+      <c r="BI1" s="1" t="inlineStr">
+        <is>
+          <t>water consumption, .1</t>
+        </is>
+      </c>
+      <c r="BJ1" s="1" t="inlineStr">
+        <is>
+          <t>ef 3.1</t>
+        </is>
+      </c>
+      <c r="BK1" s="1" t="inlineStr">
+        <is>
+          <t>acidification</t>
+        </is>
+      </c>
+      <c r="BL1" s="1" t="inlineStr">
+        <is>
+          <t>climate change</t>
+        </is>
+      </c>
+      <c r="BM1" s="1" t="inlineStr">
+        <is>
+          <t>ecotoxicity</t>
+        </is>
+      </c>
+      <c r="BN1" s="1" t="inlineStr">
+        <is>
+          <t>particulate</t>
+        </is>
+      </c>
+      <c r="BO1" s="1" t="inlineStr">
+        <is>
+          <t>eutrophication,</t>
+        </is>
+      </c>
+      <c r="BP1" s="1" t="inlineStr">
+        <is>
+          <t>eutrophication, .1</t>
+        </is>
+      </c>
+      <c r="BQ1" s="1" t="inlineStr">
+        <is>
+          <t>eutrophication,</t>
+        </is>
+      </c>
+      <c r="BR1" s="1" t="inlineStr">
+        <is>
+          <t>human toxicity,</t>
+        </is>
+      </c>
+      <c r="BS1" s="1" t="inlineStr">
+        <is>
+          <t>human toxicity, non-cancer</t>
+        </is>
+      </c>
+      <c r="BT1" s="1" t="inlineStr">
+        <is>
+          <t>ionising radiation</t>
+        </is>
+      </c>
+      <c r="BU1" s="1" t="inlineStr">
+        <is>
+          <t>land use.1</t>
+        </is>
+      </c>
+      <c r="BV1" s="1" t="inlineStr">
+        <is>
+          <t>ozone depletion</t>
+        </is>
+      </c>
+      <c r="BW1" s="1" t="inlineStr">
+        <is>
+          <t>photochemical ozone formation</t>
+        </is>
+      </c>
+      <c r="BX1" s="1" t="inlineStr">
+        <is>
+          <t>resource use,</t>
+        </is>
+      </c>
+      <c r="BY1" s="1" t="inlineStr">
+        <is>
+          <t>resource use,.1</t>
+        </is>
+      </c>
+      <c r="BZ1" s="1" t="inlineStr">
+        <is>
+          <t>water use</t>
+        </is>
+      </c>
+      <c r="CA1" s="1" t="inlineStr">
+        <is>
+          <t>traci</t>
+        </is>
+      </c>
+      <c r="CB1" s="1" t="inlineStr">
+        <is>
+          <t>traci.1</t>
+        </is>
+      </c>
+      <c r="CC1" s="1" t="inlineStr">
+        <is>
+          <t>traci.2</t>
+        </is>
+      </c>
+      <c r="CD1" s="1" t="inlineStr">
+        <is>
+          <t>traci.3</t>
+        </is>
+      </c>
+      <c r="CE1" s="1" t="inlineStr">
+        <is>
+          <t>traci.4</t>
+        </is>
+      </c>
+      <c r="CF1" s="1" t="inlineStr">
+        <is>
+          <t>traci.5</t>
+        </is>
+      </c>
+      <c r="CG1" s="1" t="inlineStr">
+        <is>
+          <t>traci.6</t>
+        </is>
+      </c>
+      <c r="CH1" s="1" t="inlineStr">
+        <is>
+          <t>traci.7</t>
+        </is>
+      </c>
+      <c r="CI1" s="1" t="inlineStr">
+        <is>
+          <t>traci.8</t>
+        </is>
+      </c>
+      <c r="CJ1" s="1" t="inlineStr">
+        <is>
+          <t>traci.9</t>
+        </is>
+      </c>
+      <c r="CK1" s="1" t="inlineStr">
+        <is>
+          <t>carbon</t>
+        </is>
+      </c>
+      <c r="CL1" s="1" t="inlineStr">
+        <is>
+          <t>pollutants</t>
+        </is>
+      </c>
+      <c r="CM1" s="1" t="inlineStr">
+        <is>
+          <t>water</t>
+        </is>
+      </c>
+      <c r="CN1" s="1" t="inlineStr">
+        <is>
+          <t>biodiversity.1</t>
+        </is>
+      </c>
+      <c r="CO1" s="1" t="inlineStr">
+        <is>
+          <t>resources</t>
+        </is>
+      </c>
+      <c r="CP1" s="1" t="inlineStr">
+        <is>
+          <t>classyfire</t>
+        </is>
+      </c>
+      <c r="CQ1" s="1" t="inlineStr">
+        <is>
+          <t>chemicals,plastics, and wood</t>
+        </is>
+      </c>
+      <c r="CR1" s="1" t="inlineStr">
+        <is>
+          <t>note:</t>
+        </is>
+      </c>
+      <c r="CS1" s="1" t="inlineStr">
+        <is>
+          <t>unnamed: 107</t>
+        </is>
+      </c>
+      <c r="CT1" s="1" t="inlineStr">
+        <is>
+          <t>unnamed: 110</t>
+        </is>
+      </c>
+      <c r="CU1" s="1" t="inlineStr">
+        <is>
+          <t>unnamed: 118</t>
+        </is>
+      </c>
+      <c r="CV1" s="1" t="inlineStr">
+        <is>
+          <t>source_file</t>
+        </is>
+      </c>
+      <c r="CW1" s="1" t="inlineStr">
         <is>
           <t>region</t>
         </is>
@@ -478,18 +953,297 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
+          <t>B.040.01.101</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
           <t>Energy, electricity general</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="E2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MJ </t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
         <is>
           <t>Electricity General Industry</t>
         </is>
       </c>
-      <c r="E2" t="n">
+      <c r="G2" t="n">
+        <v>0.026588084609</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.00077790314</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.00147571898</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.003988255489000001</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.020346207</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0.00089894787</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0.00057677111</v>
+      </c>
+      <c r="N2" t="n">
+        <v>0.00066102114</v>
+      </c>
+      <c r="O2" t="n">
+        <v>0.000116882</v>
+      </c>
+      <c r="P2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S2" t="n">
+        <v>7.6276289e-05</v>
+      </c>
+      <c r="T2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U2" t="n">
+        <v>0.0039119792</v>
+      </c>
+      <c r="V2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W2" t="n">
+        <v>0</v>
+      </c>
+      <c r="X2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y2" t="n">
         <v>0.13564138</v>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="Z2" t="n">
+        <v>2.44904</v>
+      </c>
+      <c r="AA2" t="n">
+        <v>1.5649539</v>
+      </c>
+      <c r="AB2" t="n">
+        <v>0.48391628</v>
+      </c>
+      <c r="AC2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD2" t="n">
+        <v>0.10806079</v>
+      </c>
+      <c r="AE2" t="n">
+        <v>0.19082981</v>
+      </c>
+      <c r="AF2" t="n">
+        <v>0.10127929</v>
+      </c>
+      <c r="AG2" t="n">
+        <v>0.0025575926</v>
+      </c>
+      <c r="AH2" t="n">
+        <v>0.0024027882</v>
+      </c>
+      <c r="AI2" t="n">
+        <v>0.00010893405</v>
+      </c>
+      <c r="AJ2" t="n">
+        <v>4.5870387e-05</v>
+      </c>
+      <c r="AK2" t="n">
+        <v>1.4405205e-07</v>
+      </c>
+      <c r="AL2" t="n">
+        <v>4.0286262e-10</v>
+      </c>
+      <c r="AM2" t="n">
+        <v>0.006424424</v>
+      </c>
+      <c r="AN2" t="n">
+        <v>1.258752e-07</v>
+      </c>
+      <c r="AO2" t="n">
+        <v>3.7979586e-10</v>
+      </c>
+      <c r="AP2" t="n">
+        <v>1.0376565e-14</v>
+      </c>
+      <c r="AQ2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS2" t="n">
+        <v>1.7713638e-11</v>
+      </c>
+      <c r="AT2" t="n">
+        <v>1.8159137e-08</v>
+      </c>
+      <c r="AU2" t="n">
+        <v>4.0395736e-12</v>
+      </c>
+      <c r="AV2" t="n">
+        <v>1.9016809e-11</v>
+      </c>
+      <c r="AW2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE2" t="n">
+        <v>8.5663883e-06</v>
+      </c>
+      <c r="BF2" t="n">
+        <v>0.0064158576</v>
+      </c>
+      <c r="BG2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BH2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BI2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BJ2" t="n">
+        <v>6.8175097e-06</v>
+      </c>
+      <c r="BK2" t="n">
+        <v>1.3110762e-07</v>
+      </c>
+      <c r="BL2" t="n">
+        <v>3.7820415e-06</v>
+      </c>
+      <c r="BM2" t="n">
+        <v>3.1470369e-10</v>
+      </c>
+      <c r="BN2" t="n">
+        <v>2.1261661e-07</v>
+      </c>
+      <c r="BO2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BR2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BS2" t="n">
+        <v>9.600088900000001e-10</v>
+      </c>
+      <c r="BT2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BU2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BV2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BW2" t="n">
+        <v>1.3486839e-07</v>
+      </c>
+      <c r="BX2" t="n">
+        <v>2.5556008e-06</v>
+      </c>
+      <c r="BY2" t="n">
+        <v>9.672780100000001e-14</v>
+      </c>
+      <c r="BZ2" t="n">
+        <v>0</v>
+      </c>
+      <c r="CA2" t="n">
+        <v>0</v>
+      </c>
+      <c r="CB2" t="n">
+        <v>0.13564138</v>
+      </c>
+      <c r="CC2" t="n">
+        <v>0</v>
+      </c>
+      <c r="CD2" t="n">
+        <v>8.970192800000001e-05</v>
+      </c>
+      <c r="CE2" t="n">
+        <v>3.9195298e-05</v>
+      </c>
+      <c r="CF2" t="n">
+        <v>0</v>
+      </c>
+      <c r="CG2" t="n">
+        <v>0</v>
+      </c>
+      <c r="CH2" t="n">
+        <v>8.396546500000001e-06</v>
+      </c>
+      <c r="CI2" t="n">
+        <v>0</v>
+      </c>
+      <c r="CJ2" t="n">
+        <v>0.096116761</v>
+      </c>
+      <c r="CK2" t="n">
+        <v>0.020346207</v>
+      </c>
+      <c r="CL2" t="n">
+        <v>0.00225362212</v>
+      </c>
+      <c r="CM2" t="n">
+        <v>0.00147571898</v>
+      </c>
+      <c r="CN2" t="n">
+        <v>0.00147571898</v>
+      </c>
+      <c r="CO2" t="n">
+        <v>0.003988255489000001</v>
+      </c>
+      <c r="CP2" t="inlineStr"/>
+      <c r="CQ2" t="inlineStr"/>
+      <c r="CR2" t="inlineStr"/>
+      <c r="CS2" t="inlineStr"/>
+      <c r="CT2" t="inlineStr"/>
+      <c r="CU2" t="inlineStr"/>
+      <c r="CV2" t="inlineStr">
+        <is>
+          <t>electricity general industry.xlsx</t>
+        </is>
+      </c>
+      <c r="CW2" t="inlineStr">
         <is>
           <t>Global</t>
         </is>
@@ -508,18 +1262,297 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
+          <t>B.040.01.104</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
           <t>Energy, electricity general</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="E3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MJ </t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
         <is>
           <t>Electricity General domestic use Low Voltage</t>
         </is>
       </c>
-      <c r="E3" t="n">
+      <c r="G3" t="n">
+        <v>0.02798745754</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.00081884541</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.0015533884</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.00419816373</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0.02141706</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0.00094626091</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0.0006071274900000001</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0.00069581173</v>
+      </c>
+      <c r="O3" t="n">
+        <v>0.00012303368</v>
+      </c>
+      <c r="P3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>0</v>
+      </c>
+      <c r="R3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S3" t="n">
+        <v>8.029083e-05</v>
+      </c>
+      <c r="T3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U3" t="n">
+        <v>0.0041178729</v>
+      </c>
+      <c r="V3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W3" t="n">
+        <v>0</v>
+      </c>
+      <c r="X3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y3" t="n">
         <v>0.1427804</v>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="Z3" t="n">
+        <v>2.5779369</v>
+      </c>
+      <c r="AA3" t="n">
+        <v>1.6473199</v>
+      </c>
+      <c r="AB3" t="n">
+        <v>0.50938556</v>
+      </c>
+      <c r="AC3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD3" t="n">
+        <v>0.1137482</v>
+      </c>
+      <c r="AE3" t="n">
+        <v>0.20087348</v>
+      </c>
+      <c r="AF3" t="n">
+        <v>0.10660978</v>
+      </c>
+      <c r="AG3" t="n">
+        <v>0.0026922027</v>
+      </c>
+      <c r="AH3" t="n">
+        <v>0.0025292507</v>
+      </c>
+      <c r="AI3" t="n">
+        <v>0.00011466742</v>
+      </c>
+      <c r="AJ3" t="n">
+        <v>4.8284618e-05</v>
+      </c>
+      <c r="AK3" t="n">
+        <v>1.5163374e-07</v>
+      </c>
+      <c r="AL3" t="n">
+        <v>4.2406591e-10</v>
+      </c>
+      <c r="AM3" t="n">
+        <v>0.0067625516</v>
+      </c>
+      <c r="AN3" t="n">
+        <v>1.3250021e-07</v>
+      </c>
+      <c r="AO3" t="n">
+        <v>3.9978511e-10</v>
+      </c>
+      <c r="AP3" t="n">
+        <v>1.09227e-14</v>
+      </c>
+      <c r="AQ3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS3" t="n">
+        <v>1.8645935e-11</v>
+      </c>
+      <c r="AT3" t="n">
+        <v>1.9114881e-08</v>
+      </c>
+      <c r="AU3" t="n">
+        <v>4.2521828e-12</v>
+      </c>
+      <c r="AV3" t="n">
+        <v>2.0017693e-11</v>
+      </c>
+      <c r="AW3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ3" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA3" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB3" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC3" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD3" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE3" t="n">
+        <v>9.0172508e-06</v>
+      </c>
+      <c r="BF3" t="n">
+        <v>0.0067535343</v>
+      </c>
+      <c r="BG3" t="n">
+        <v>0</v>
+      </c>
+      <c r="BH3" t="n">
+        <v>0</v>
+      </c>
+      <c r="BI3" t="n">
+        <v>0</v>
+      </c>
+      <c r="BJ3" t="n">
+        <v>7.176326e-06</v>
+      </c>
+      <c r="BK3" t="n">
+        <v>1.3800803e-07</v>
+      </c>
+      <c r="BL3" t="n">
+        <v>3.9810963e-06</v>
+      </c>
+      <c r="BM3" t="n">
+        <v>3.3126704e-10</v>
+      </c>
+      <c r="BN3" t="n">
+        <v>2.2380696e-07</v>
+      </c>
+      <c r="BO3" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP3" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ3" t="n">
+        <v>0</v>
+      </c>
+      <c r="BR3" t="n">
+        <v>0</v>
+      </c>
+      <c r="BS3" t="n">
+        <v>1.0105357e-09</v>
+      </c>
+      <c r="BT3" t="n">
+        <v>0</v>
+      </c>
+      <c r="BU3" t="n">
+        <v>0</v>
+      </c>
+      <c r="BV3" t="n">
+        <v>0</v>
+      </c>
+      <c r="BW3" t="n">
+        <v>1.4196673e-07</v>
+      </c>
+      <c r="BX3" t="n">
+        <v>2.6901061e-06</v>
+      </c>
+      <c r="BY3" t="n">
+        <v>1.0181874e-13</v>
+      </c>
+      <c r="BZ3" t="n">
+        <v>0</v>
+      </c>
+      <c r="CA3" t="n">
+        <v>0</v>
+      </c>
+      <c r="CB3" t="n">
+        <v>0.1427804</v>
+      </c>
+      <c r="CC3" t="n">
+        <v>0</v>
+      </c>
+      <c r="CD3" t="n">
+        <v>9.4423082e-05</v>
+      </c>
+      <c r="CE3" t="n">
+        <v>4.1258208e-05</v>
+      </c>
+      <c r="CF3" t="n">
+        <v>0</v>
+      </c>
+      <c r="CG3" t="n">
+        <v>0</v>
+      </c>
+      <c r="CH3" t="n">
+        <v>8.83847e-06</v>
+      </c>
+      <c r="CI3" t="n">
+        <v>0</v>
+      </c>
+      <c r="CJ3" t="n">
+        <v>0.10117554</v>
+      </c>
+      <c r="CK3" t="n">
+        <v>0.02141706</v>
+      </c>
+      <c r="CL3" t="n">
+        <v>0.00237223381</v>
+      </c>
+      <c r="CM3" t="n">
+        <v>0.0015533884</v>
+      </c>
+      <c r="CN3" t="n">
+        <v>0.0015533884</v>
+      </c>
+      <c r="CO3" t="n">
+        <v>0.00419816373</v>
+      </c>
+      <c r="CP3" t="inlineStr"/>
+      <c r="CQ3" t="inlineStr"/>
+      <c r="CR3" t="inlineStr"/>
+      <c r="CS3" t="inlineStr"/>
+      <c r="CT3" t="inlineStr"/>
+      <c r="CU3" t="inlineStr"/>
+      <c r="CV3" t="inlineStr">
+        <is>
+          <t>electricity general industry.xlsx</t>
+        </is>
+      </c>
+      <c r="CW3" t="inlineStr">
         <is>
           <t>Global</t>
         </is>

</xml_diff>